<commit_message>
Criar função para estilizar tabela do Excel.
</commit_message>
<xml_diff>
--- a/test/Ofertas.xlsx
+++ b/test/Ofertas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="list_offers" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,15 +26,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004682B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B0E0E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,10 +68,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,13 +444,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="105.6" customWidth="1" min="1" max="1"/>
+    <col width="8.4" customWidth="1" min="2" max="2"/>
+    <col width="254.4" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -451,135 +475,120 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>apple iphone 12 64gb 5g - 12mp ios - tela super retina xdr oled 6.1" - branco</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>3496</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21015&amp;parceiro=8926&amp;srsltid=AfmBOoqVk47Y3rLb_n8ILWstTVPZzhJ_2mltmUfKT_ZhJzMoDYZhq8Kpczs</t>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21015&amp;parceiro=8926&amp;srsltid=AfmBOop7QT2QWzfffc3ucPr5qDv5-LBulEBemOo_Mld2rkLZH9PbqStehME</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>apple iphone 12 preto 64gb</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="3" t="n">
         <v>3130</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>https://doji.com.br/product/apple-iphone-12-preto-64gb-como-novo</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>usado: iphone 12 64gb azul excelente - trocafone - apple</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3343.12</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-excelente-trocafone-apple/p/cd5jh8ej67/te/ceba?&amp;seller_id=trocafone</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>celular iphone 12 5g 64gb azul - open box</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3305.22</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>https://www.maisbaratofone.com.br/produto/celular-apple-iphone-12-5g/?attribute_pa_condicao=open-box&amp;attribute_pa_armazenamento=64gb&amp;attribute_pa_cor=azul</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3379.9</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p</t>
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>iphone 11 apple 64gb e 128gb preto 6,1” 12mp ios (64gb)</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>3399</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>https://lumixpel.lojavirtualnuvem.com.br/produtos/iphone-11-apple-64gb-e-128gb-preto-61-12mp-ios/?variant=660570516&amp;pf=mc&amp;srsltid=AfmBOoqziRKAjMUfbeedAm2fxGcT81D2QWVcDj6mplup1knjq7qw1D91WX8</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3349</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p</t>
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ailos aproxima | iphone 12 64gb azul - swap</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>3424</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>https://ailosaproxima.coop.br/loja/malibu-shop/produto/380030/iphone-12-64gb-azul-swap</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>celular apple iphone 12 white 64gb vitrine/seminovo + acessorios</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>3499</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p</t>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>3039</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>3289.9</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p</t>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>pc gamer ryzen 5 5500 + rtx 3060ti 8gb + 16gb ram + gb1713</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>4399</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>https://www.newyorkinformatica.com.br/pc-gamer-ryzen-5-5500-rtx-3060ti-8gb-16gb-ram-gb1713</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>smartphone apple iphone 12 64gb câmera dupla</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>3039</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 192 bits asus dual-rtx3060ti-o8g-v2</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B9" s="3" t="n">
         <v>4108.27</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-ti-8-gb-gddr6-192-bits-asus-dual-rtx3060ti-o8g-v2?_lc=88&amp;searchterm=rtx%203060</t>
         </is>

</xml_diff>

<commit_message>
Enviar e-mail com o(s) produto(s) encontrado(s) na faixa de preço desejada.
</commit_message>
<xml_diff>
--- a/test/Ofertas.xlsx
+++ b/test/Ofertas.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,118 +477,178 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>apple iphone 12 64gb 5g - 12mp ios - tela super retina xdr oled 6.1" - branco</t>
+          <t>usado: iphone 12 64gb azul bom - trocafone - apple</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>3496</v>
+        <v>3483.92</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21015&amp;parceiro=8926&amp;srsltid=AfmBOop7QT2QWzfffc3ucPr5qDv5-LBulEBemOo_Mld2rkLZH9PbqStehME</t>
+          <t>https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-bom-trocafone-apple/p/djccka1jka/te/ip12?&amp;seller_id=trocafone</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>apple iphone 12 preto 64gb</t>
+          <t>celular iphone 12 5g 64gb azul - open box</t>
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>3130</v>
+        <v>3305.22</v>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>https://doji.com.br/product/apple-iphone-12-preto-64gb-como-novo</t>
+          <t>https://www.maisbaratofone.com.br/produto/celular-apple-iphone-12-5g/?attribute_pa_condicao=open-box&amp;attribute_pa_armazenamento=64gb&amp;attribute_pa_cor=azul</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>celular iphone 12 5g 64gb azul - open box</t>
+          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3305.22</v>
+        <v>3349</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>https://www.maisbaratofone.com.br/produto/celular-apple-iphone-12-5g/?attribute_pa_condicao=open-box&amp;attribute_pa_armazenamento=64gb&amp;attribute_pa_cor=azul</t>
+          <t>https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>iphone 11 apple 64gb e 128gb preto 6,1” 12mp ios (64gb)</t>
+          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>3399</v>
+        <v>3379.9</v>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>https://lumixpel.lojavirtualnuvem.com.br/produtos/iphone-11-apple-64gb-e-128gb-preto-61-12mp-ios/?variant=660570516&amp;pf=mc&amp;srsltid=AfmBOoqziRKAjMUfbeedAm2fxGcT81D2QWVcDj6mplup1knjq7qw1D91WX8</t>
+          <t>https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>ailos aproxima | iphone 12 64gb azul - swap</t>
+          <t>apple iphone 12 preto 64gb</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>3424</v>
+        <v>3130</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>https://ailosaproxima.coop.br/loja/malibu-shop/produto/380030/iphone-12-64gb-azul-swap</t>
+          <t>https://doji.com.br/product/apple-iphone-12-preto-64gb-como-novo</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+          <t>iphone 12 64gb | celular apple | usado</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>3039</v>
+        <v>3015</v>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
+          <t>https://www.enjoei.com.br/p/iphone-12-64gb-87683383?g_campaign=google_shopping</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>pc gamer ryzen 5 5500 + rtx 3060ti 8gb + 16gb ram + gb1713</t>
+          <t>celular apple iphone 12 white 64gb vitrine/seminovo + acessorios</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4399</v>
+        <v>3499</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>https://www.newyorkinformatica.com.br/pc-gamer-ryzen-5-5500-rtx-3060ti-8gb-16gb-ram-gb1713</t>
+          <t>https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
+          <t>apple iphone 12 64gb 5g - 12mp ios - tela super retina xdr oled 6.1" - preto</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>3496</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21019&amp;parceiro=8926&amp;srsltid=AfmBOoozsDDR7IV2lzsIi-H9hEmjiMHREVqc1qljiZcBUvg6fMHPQX9JPnE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>3289.9</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>iphone 11 apple 64gb e 128gb preto 6,1” 12mp ios (64gb)</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>3399</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>https://lumixpel.lojavirtualnuvem.com.br/produtos/iphone-11-apple-64gb-e-128gb-preto-61-12mp-ios/?variant=660570516&amp;pf=mc&amp;srsltid=AfmBOor-FQ3Bwl67FXC1WlzVEsKcidTQI9oQc4rijmidm1cBfqeMVbo2Jns</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>3199</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
           <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 192 bits asus dual-rtx3060ti-o8g-v2</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B13" s="3" t="n">
         <v>4108.27</v>
       </c>
-      <c r="C9" s="3" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-ti-8-gb-gddr6-192-bits-asus-dual-rtx3060ti-o8g-v2?_lc=88&amp;searchterm=rtx%203060</t>
         </is>

</xml_diff>

<commit_message>
Verificar se existe alguma oferta dentro da tabela de ofertas.
</commit_message>
<xml_diff>
--- a/test/Ofertas.xlsx
+++ b/test/Ofertas.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21019&amp;parceiro=8926&amp;srsltid=AfmBOoozsDDR7IV2lzsIi-H9hEmjiMHREVqc1qljiZcBUvg6fMHPQX9JPnE</t>
+          <t>https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1?variant_id=21019&amp;parceiro=8926&amp;srsltid=AfmBOopqbiO0i-O8ok7RtRlBKV1bYVWIvzNe224FJHUrq61-q-tWbwQ2CIU</t>
         </is>
       </c>
     </row>
@@ -620,35 +620,50 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>https://lumixpel.lojavirtualnuvem.com.br/produtos/iphone-11-apple-64gb-e-128gb-preto-61-12mp-ios/?variant=660570516&amp;pf=mc&amp;srsltid=AfmBOor-FQ3Bwl67FXC1WlzVEsKcidTQI9oQc4rijmidm1cBfqeMVbo2Jns</t>
+          <t>https://lumixpel.lojavirtualnuvem.com.br/produtos/iphone-11-apple-64gb-e-128gb-preto-61-12mp-ios/?variant=660570516&amp;pf=mc&amp;srsltid=AfmBOop3hX52tE7OjosJ4QLXIMq4G1OmpC0TR4CEadcctajK-hJ_gyFcm70</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+          <t>ailos aproxima | iphone 12 64gb azul - swap</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>3199</v>
+        <v>3424</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
+          <t>https://ailosaproxima.coop.br/loja/malibu-shop/produto/380030/iphone-12-64gb-azul-swap</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
+          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>3039</v>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
           <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 192 bits asus dual-rtx3060ti-o8g-v2</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B14" s="2" t="n">
         <v>4108.27</v>
       </c>
-      <c r="C13" s="3" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-ti-8-gb-gddr6-192-bits-asus-dual-rtx3060ti-o8g-v2?_lc=88&amp;searchterm=rtx%203060</t>
         </is>

</xml_diff>